<commit_message>
Nueva base de datos. Ya tegno completa la parte de las estadísticas. Revisar ToDo.txt
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\PycharmProjects\nba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0D8D546-6DDF-4208-8EC3-A58738F7E751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF17552-FA4B-4A7D-83C1-8D1873041DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{7E229403-3AC3-40FF-B32A-0CABDA96EFD3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="22">
   <si>
     <t>Home</t>
   </si>
@@ -73,13 +73,43 @@
   <si>
     <t>W</t>
   </si>
+  <si>
+    <t xml:space="preserve">General </t>
+  </si>
+  <si>
+    <t>General Home</t>
+  </si>
+  <si>
+    <t>Q_1 Home</t>
+  </si>
+  <si>
+    <t>Q_2 Home</t>
+  </si>
+  <si>
+    <t>Q_3 Home</t>
+  </si>
+  <si>
+    <t>Q_4 Home</t>
+  </si>
+  <si>
+    <t>Q_1 Away</t>
+  </si>
+  <si>
+    <t>Q_2 Away</t>
+  </si>
+  <si>
+    <t>Q_3 Away</t>
+  </si>
+  <si>
+    <t>Q_4 Away</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -133,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -147,13 +177,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -8242,10 +8266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D021EF-9853-4E60-9C8B-7CA3B6CAEC4F}">
-  <dimension ref="B2:O33"/>
+  <dimension ref="B2:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8259,7 +8283,7 @@
     <col min="14" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
@@ -8275,7 +8299,7 @@
       <c r="H2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="2">
         <v>10</v>
       </c>
       <c r="K2" s="3" t="s">
@@ -8288,7 +8312,7 @@
       </c>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -8326,7 +8350,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -8358,7 +8382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -8397,7 +8421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -8429,7 +8453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -8461,7 +8485,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -8493,7 +8517,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -8525,7 +8549,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -8557,7 +8581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -8589,7 +8613,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -8621,7 +8645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -8653,7 +8677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -8685,7 +8709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -8717,7 +8741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -8748,8 +8772,11 @@
       <c r="O16" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="Q16" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -8780,8 +8807,11 @@
       <c r="O17" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="Q17" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -8812,8 +8842,11 @@
       <c r="O18" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="Q18" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -8845,7 +8878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -8876,8 +8909,11 @@
       <c r="O20" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="Q20" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -8908,8 +8944,11 @@
       <c r="O21" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="Q21" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>20</v>
       </c>
@@ -8940,8 +8979,11 @@
       <c r="O22" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="Q22" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>21</v>
       </c>
@@ -8972,8 +9014,11 @@
       <c r="O23" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="Q23" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>22</v>
       </c>
@@ -9005,7 +9050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>23</v>
       </c>
@@ -9036,8 +9081,11 @@
       <c r="O25" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="Q25" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>24</v>
       </c>
@@ -9068,8 +9116,11 @@
       <c r="O26" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="Q26" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>25</v>
       </c>
@@ -9100,9 +9151,12 @@
       <c r="O27" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="Q27" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="G28" s="6"/>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="G28" s="5"/>
       <c r="K28" s="2">
         <v>71</v>
       </c>
@@ -9116,8 +9170,11 @@
       <c r="O28" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="Q28" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E30" s="2" t="s">
         <v>6</v>
       </c>
@@ -9126,22 +9183,21 @@
         <v>4.0750000000000002</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L30" s="2">
-        <f>MEDIAN(K3:K28)</f>
-        <v>83.5</v>
-      </c>
-      <c r="M30" s="7"/>
+        <f>AVERAGE(K3:K28)</f>
+        <v>82.269230769230774</v>
+      </c>
       <c r="N30" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O30" s="2">
-        <f>MEDIAN(N3:N28)</f>
-        <v>82</v>
+        <f>AVERAGE(N3:N28)</f>
+        <v>84.65384615384616</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E31" s="2" t="s">
         <v>7</v>
       </c>
@@ -9150,22 +9206,21 @@
         <v>4.1150000000000002</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L31" s="2">
-        <f>AVERAGE(K3:K28)</f>
-        <v>82.269230769230774</v>
-      </c>
-      <c r="M31" s="7"/>
+        <f>MEDIAN(K3:K28)</f>
+        <v>83.5</v>
+      </c>
       <c r="N31" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O31" s="2">
-        <f>AVERAGE(N3:N28)</f>
-        <v>84.65384615384616</v>
+        <f>MEDIAN(N3:N28)</f>
+        <v>82</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E32" s="2" t="s">
         <v>8</v>
       </c>
@@ -9180,7 +9235,6 @@
         <f>MAX(K3:K28)</f>
         <v>108</v>
       </c>
-      <c r="M32" s="7"/>
       <c r="N32" s="2" t="s">
         <v>8</v>
       </c>
@@ -9204,7 +9258,6 @@
         <f>MIN(K3:K28)</f>
         <v>56</v>
       </c>
-      <c r="M33" s="7"/>
       <c r="N33" s="2" t="s">
         <v>9</v>
       </c>

</xml_diff>